<commit_message>
Fixed inability to pass in duplicate asset descriptions as input
</commit_message>
<xml_diff>
--- a/model_inputs/financial_reports/clinical/FHA.xlsx
+++ b/model_inputs/financial_reports/clinical/FHA.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84524928-2AC7-4E58-88C0-1917F9F5C82E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="13"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="4" r:id="rId1"/>
@@ -22,7 +23,17 @@
     <sheet name="BME_FCH" sheetId="25" r:id="rId13"/>
     <sheet name="BME_POC" sheetId="26" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -86,7 +97,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0;\(#,##0\)"/>
@@ -299,6 +310,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -334,6 +362,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -509,7 +554,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -559,11 +604,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="C5" sqref="C5:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +666,7 @@
         <v>1313</v>
       </c>
       <c r="B2" s="7">
-        <f>C2-D2-E2-F2</f>
+        <f>C2-D2</f>
         <v>47633.3</v>
       </c>
       <c r="C2" s="8">
@@ -633,7 +678,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="8"/>
       <c r="G2" s="7">
-        <f>H2-I2-J2-K2</f>
+        <f>H2-I2</f>
         <v>47558</v>
       </c>
       <c r="H2" s="8">
@@ -650,7 +695,7 @@
         <v>1413</v>
       </c>
       <c r="B3" s="7">
-        <f t="shared" ref="B3:B9" si="0">C3-D3-E3-F3</f>
+        <f t="shared" ref="B3:B9" si="0">C3-D3</f>
         <v>53259.31</v>
       </c>
       <c r="C3" s="8">
@@ -662,7 +707,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="8"/>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G9" si="1">H3-I3-J3-K3</f>
+        <f t="shared" ref="G3:G9" si="1">H3-I3</f>
         <v>49408</v>
       </c>
       <c r="H3" s="8">
@@ -854,11 +899,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,7 +961,7 @@
         <v>1313</v>
       </c>
       <c r="B2" s="7">
-        <f>C2-D2-E2-F2</f>
+        <f>C2-D2</f>
         <v>147799.16999999998</v>
       </c>
       <c r="C2" s="8">
@@ -928,7 +973,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="8"/>
       <c r="G2" s="7">
-        <f>H2-I2-J2-K2</f>
+        <f>H2-I2</f>
         <v>128462</v>
       </c>
       <c r="H2" s="8">
@@ -945,7 +990,7 @@
         <v>1413</v>
       </c>
       <c r="B3" s="7">
-        <f t="shared" ref="B3:B9" si="0">C3-D3-E3-F3</f>
+        <f t="shared" ref="B3:B9" si="0">C3-D3</f>
         <v>169082.83000000002</v>
       </c>
       <c r="C3" s="8">
@@ -957,7 +1002,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="8"/>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G9" si="1">H3-I3-J3-K3</f>
+        <f t="shared" ref="G3:G9" si="1">H3-I3</f>
         <v>133365</v>
       </c>
       <c r="H3" s="8">
@@ -1149,11 +1194,11 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,7 +1256,7 @@
         <v>1313</v>
       </c>
       <c r="B2" s="7">
-        <f>C2-D2-E2-F2</f>
+        <f>C2-D2</f>
         <v>243911.78999999998</v>
       </c>
       <c r="C2" s="8">
@@ -1223,7 +1268,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="8"/>
       <c r="G2" s="7">
-        <f>H2-I2-J2-K2</f>
+        <f>H2-I2</f>
         <v>243665</v>
       </c>
       <c r="H2" s="8">
@@ -1240,7 +1285,7 @@
         <v>1413</v>
       </c>
       <c r="B3" s="7">
-        <f t="shared" ref="B3:B9" si="0">C3-D3-E3-F3</f>
+        <f t="shared" ref="B3:B9" si="0">C3-D3</f>
         <v>290885.04000000004</v>
       </c>
       <c r="C3" s="8">
@@ -1252,7 +1297,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="8"/>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G9" si="1">H3-I3-J3-K3</f>
+        <f t="shared" ref="G3:G9" si="1">H3-I3</f>
         <v>288801</v>
       </c>
       <c r="H3" s="8">
@@ -1444,11 +1489,11 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K9"/>
+      <selection activeCell="G2" sqref="G2:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,7 +1551,7 @@
         <v>1313</v>
       </c>
       <c r="B2" s="7">
-        <f>C2-D2-E2-F2</f>
+        <f>C2-D2</f>
         <v>14530.6</v>
       </c>
       <c r="C2" s="8">
@@ -1518,7 +1563,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="8"/>
       <c r="G2" s="7">
-        <f>H2-I2-J2-K2</f>
+        <f>H2-I2</f>
         <v>14530.6</v>
       </c>
       <c r="H2" s="8">
@@ -1535,7 +1580,7 @@
         <v>1413</v>
       </c>
       <c r="B3" s="7">
-        <f t="shared" ref="B3:B9" si="0">C3-D3-E3-F3</f>
+        <f t="shared" ref="B3:B9" si="0">C3-D3</f>
         <v>15099</v>
       </c>
       <c r="C3" s="8">
@@ -1547,7 +1592,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="8"/>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G9" si="1">H3-I3-J3-K3</f>
+        <f t="shared" ref="G3:G9" si="1">H3-I3</f>
         <v>15099</v>
       </c>
       <c r="H3" s="8">
@@ -1739,11 +1784,11 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1801,7 +1846,7 @@
         <v>1213</v>
       </c>
       <c r="B2" s="7">
-        <f>C2-D2-E2-F2</f>
+        <f>C2-D2</f>
         <v>387445.54</v>
       </c>
       <c r="C2" s="8">
@@ -1813,7 +1858,7 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
       <c r="G2" s="7">
-        <f>H2-I2-J2-K2</f>
+        <f>H2-I2</f>
         <v>362364</v>
       </c>
       <c r="H2" s="8">
@@ -1830,7 +1875,7 @@
         <v>1313</v>
       </c>
       <c r="B3" s="7">
-        <f>C3-D3-E3-F3</f>
+        <f t="shared" ref="B3:B10" si="0">C3-D3</f>
         <v>332053.07000000007</v>
       </c>
       <c r="C3" s="8">
@@ -1842,7 +1887,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="8"/>
       <c r="G3" s="7">
-        <f>H3-I3-J3-K3</f>
+        <f t="shared" ref="G3:G10" si="1">H3-I3</f>
         <v>1297235</v>
       </c>
       <c r="H3" s="8">
@@ -1859,7 +1904,7 @@
         <v>1413</v>
       </c>
       <c r="B4" s="7">
-        <f t="shared" ref="B4:B10" si="0">C4-D4-E4-F4</f>
+        <f t="shared" si="0"/>
         <v>268115.15000000002</v>
       </c>
       <c r="C4" s="8">
@@ -1871,7 +1916,7 @@
       <c r="E4" s="9"/>
       <c r="F4" s="8"/>
       <c r="G4" s="7">
-        <f t="shared" ref="G4:G10" si="1">H4-I4-J4-K4</f>
+        <f t="shared" si="1"/>
         <v>1005688</v>
       </c>
       <c r="H4" s="8">
@@ -2063,11 +2108,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2135,7 +2180,7 @@
         <v>1313</v>
       </c>
       <c r="B2" s="7">
-        <f>C2-D2-E2-F2</f>
+        <f>C2-D2</f>
         <v>109698.68999999997</v>
       </c>
       <c r="C2" s="8">
@@ -2147,7 +2192,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="8"/>
       <c r="G2" s="7">
-        <f>H2-I2-J2-K2</f>
+        <f>H2-I2</f>
         <v>118808</v>
       </c>
       <c r="H2" s="8">
@@ -2164,7 +2209,7 @@
         <v>1413</v>
       </c>
       <c r="B3" s="7">
-        <f t="shared" ref="B3:B9" si="0">C3-D3-E3-F3</f>
+        <f t="shared" ref="B3:B9" si="0">C3-D3</f>
         <v>140388.09999999998</v>
       </c>
       <c r="C3" s="8">
@@ -2176,7 +2221,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="8"/>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G9" si="1">H3-I3-J3-K3</f>
+        <f t="shared" ref="G3:G9" si="1">H3-I3</f>
         <v>123294</v>
       </c>
       <c r="H3" s="8">
@@ -2385,11 +2430,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2447,7 +2492,7 @@
         <v>1313</v>
       </c>
       <c r="B2" s="7">
-        <f>C2-D2-E2-F2</f>
+        <f>C2-D2</f>
         <v>478500.73</v>
       </c>
       <c r="C2" s="8">
@@ -2459,7 +2504,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="8"/>
       <c r="G2" s="7">
-        <f>H2-I2-J2-K2</f>
+        <f>H2-I2</f>
         <v>480223</v>
       </c>
       <c r="H2" s="8">
@@ -2476,7 +2521,7 @@
         <v>1413</v>
       </c>
       <c r="B3" s="7">
-        <f t="shared" ref="B3:B9" si="0">C3-D3-E3-F3</f>
+        <f t="shared" ref="B3:B9" si="0">C3-D3</f>
         <v>563516.02000000014</v>
       </c>
       <c r="C3" s="8">
@@ -2488,7 +2533,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="8"/>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G9" si="1">H3-I3-J3-K3</f>
+        <f t="shared" ref="G3:G9" si="1">H3-I3</f>
         <v>496876</v>
       </c>
       <c r="H3" s="8">
@@ -2680,11 +2725,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K9"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2742,7 +2787,7 @@
         <v>1313</v>
       </c>
       <c r="B2" s="7">
-        <f>C2-D2-E2-F2</f>
+        <f>C2-D2</f>
         <v>84318.270000000019</v>
       </c>
       <c r="C2" s="8">
@@ -2754,7 +2799,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="8"/>
       <c r="G2" s="7">
-        <f>H2-I2-J2-K2</f>
+        <f>H2-I2</f>
         <v>81874</v>
       </c>
       <c r="H2" s="8">
@@ -2771,7 +2816,7 @@
         <v>1413</v>
       </c>
       <c r="B3" s="7">
-        <f t="shared" ref="B3:B9" si="0">C3-D3-E3-F3</f>
+        <f t="shared" ref="B3:B9" si="0">C3-D3</f>
         <v>96079.62</v>
       </c>
       <c r="C3" s="8">
@@ -2783,7 +2828,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="8"/>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G9" si="1">H3-I3-J3-K3</f>
+        <f t="shared" ref="G3:G9" si="1">H3-I3</f>
         <v>86951</v>
       </c>
       <c r="H3" s="8">
@@ -2975,11 +3020,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3037,7 +3082,7 @@
         <v>1313</v>
       </c>
       <c r="B2" s="7">
-        <f>C2-D2-E2-F2</f>
+        <f>C2-D2</f>
         <v>197744.12999999998</v>
       </c>
       <c r="C2" s="8">
@@ -3049,7 +3094,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="8"/>
       <c r="G2" s="7">
-        <f>H2-I2-J2-K2</f>
+        <f>H2-I2</f>
         <v>89211</v>
       </c>
       <c r="H2" s="8">
@@ -3066,7 +3111,7 @@
         <v>1413</v>
       </c>
       <c r="B3" s="7">
-        <f t="shared" ref="B3:B9" si="0">C3-D3-E3-F3</f>
+        <f t="shared" ref="B3:B9" si="0">C3-D3</f>
         <v>217908.21999999997</v>
       </c>
       <c r="C3" s="8">
@@ -3078,7 +3123,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="8"/>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G9" si="1">H3-I3-J3-K3</f>
+        <f t="shared" ref="G3:G9" si="1">H3-I3</f>
         <v>94680</v>
       </c>
       <c r="H3" s="8">
@@ -3270,11 +3315,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3332,7 +3377,7 @@
         <v>1313</v>
       </c>
       <c r="B2" s="7">
-        <f>C2-D2-E2-F2</f>
+        <f>C2-D2</f>
         <v>175119.77000000002</v>
       </c>
       <c r="C2" s="8">
@@ -3344,7 +3389,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="8"/>
       <c r="G2" s="7">
-        <f>H2-I2-J2-K2</f>
+        <f>H2-I2</f>
         <v>195758</v>
       </c>
       <c r="H2" s="8">
@@ -3361,7 +3406,7 @@
         <v>1413</v>
       </c>
       <c r="B3" s="7">
-        <f t="shared" ref="B3:B9" si="0">C3-D3-E3-F3</f>
+        <f t="shared" ref="B3:B9" si="0">C3-D3</f>
         <v>210431.43000000005</v>
       </c>
       <c r="C3" s="8">
@@ -3373,7 +3418,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="8"/>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G9" si="1">H3-I3-J3-K3</f>
+        <f t="shared" ref="G3:G9" si="1">H3-I3</f>
         <v>203283</v>
       </c>
       <c r="H3" s="8">
@@ -3565,11 +3610,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K9"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3627,7 +3672,7 @@
         <v>1313</v>
       </c>
       <c r="B2" s="7">
-        <f>C2-D2-E2-F2</f>
+        <f>C2-D2</f>
         <v>410553.62999999989</v>
       </c>
       <c r="C2" s="8">
@@ -3639,7 +3684,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="8"/>
       <c r="G2" s="7">
-        <f>H2-I2-J2-K2</f>
+        <f>H2-I2</f>
         <v>400790</v>
       </c>
       <c r="H2" s="8">
@@ -3656,7 +3701,7 @@
         <v>1413</v>
       </c>
       <c r="B3" s="7">
-        <f t="shared" ref="B3:B9" si="0">C3-D3-E3-F3</f>
+        <f t="shared" ref="B3:B9" si="0">C3-D3</f>
         <v>493571.49</v>
       </c>
       <c r="C3" s="8">
@@ -3668,7 +3713,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="8"/>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G9" si="1">H3-I3-J3-K3</f>
+        <f t="shared" ref="G3:G9" si="1">H3-I3</f>
         <v>386401.25</v>
       </c>
       <c r="H3" s="8">
@@ -3860,11 +3905,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3922,7 +3967,7 @@
         <v>1313</v>
       </c>
       <c r="B2" s="7">
-        <f>C2-D2-E2-F2</f>
+        <f>C2-D2</f>
         <v>65624.61</v>
       </c>
       <c r="C2" s="8">
@@ -3934,7 +3979,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="8"/>
       <c r="G2" s="7">
-        <f>H2-I2-J2-K2</f>
+        <f>H2-I2</f>
         <v>61119</v>
       </c>
       <c r="H2" s="8">
@@ -3951,7 +3996,7 @@
         <v>1413</v>
       </c>
       <c r="B3" s="7">
-        <f t="shared" ref="B3:B9" si="0">C3-D3-E3-F3</f>
+        <f t="shared" ref="B3:B9" si="0">C3-D3</f>
         <v>80750.929999999993</v>
       </c>
       <c r="C3" s="8">
@@ -3963,7 +4008,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="8"/>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G9" si="1">H3-I3-J3-K3</f>
+        <f t="shared" ref="G3:G9" si="1">H3-I3</f>
         <v>63386</v>
       </c>
       <c r="H3" s="8">
@@ -4155,11 +4200,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K9"/>
+      <selection activeCell="G2" sqref="G2:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4217,7 +4262,7 @@
         <v>1313</v>
       </c>
       <c r="B2" s="7">
-        <f>C2-D2-E2-F2</f>
+        <f>C2-D2</f>
         <v>214791.89</v>
       </c>
       <c r="C2" s="8">
@@ -4229,7 +4274,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="8"/>
       <c r="G2" s="7">
-        <f>H2-I2-J2-K2</f>
+        <f>H2-I2</f>
         <v>133003</v>
       </c>
       <c r="H2" s="8">
@@ -4246,7 +4291,7 @@
         <v>1413</v>
       </c>
       <c r="B3" s="7">
-        <f t="shared" ref="B3:B9" si="0">C3-D3-E3-F3</f>
+        <f t="shared" ref="B3:B9" si="0">C3-D3</f>
         <v>267623.44999999995</v>
       </c>
       <c r="C3" s="8">
@@ -4258,7 +4303,7 @@
       <c r="E3" s="9"/>
       <c r="F3" s="8"/>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G9" si="1">H3-I3-J3-K3</f>
+        <f t="shared" ref="G3:G9" si="1">H3-I3</f>
         <v>144540</v>
       </c>
       <c r="H3" s="8">

</xml_diff>